<commit_message>
terceiro commit: ajuste dos dados
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rubens Pereira\Documents\RUBENS\PROJETOS\geomap-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F526EE27-8BA3-41DF-9680-DE56D9B68B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CCD322-DD61-4C9D-8F98-43C7BD0F878E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{2FA2D2D9-05F8-4A7A-8715-5A3A81492CDF}"/>
   </bookViews>
@@ -11411,8 +11411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B975A1-6E88-43A0-B6E9-1A1207B94735}">
   <dimension ref="A1:O1279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A815" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J839" sqref="J839"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12287,7 +12287,7 @@
         <v>52</v>
       </c>
       <c r="J22" s="11">
-        <v>40400000</v>
+        <v>49400000</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>14</v>

</xml_diff>